<commit_message>
Latest Changes Push By Naveen
</commit_message>
<xml_diff>
--- a/fms/donations_report.xlsx
+++ b/fms/donations_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,35 +441,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Item No</t>
+          <t>Item Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Item Name</t>
+          <t>Item Type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Item Type</t>
+          <t>Calories</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Calories</t>
+          <t>Amount (lb)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Amount (lb)</t>
+          <t>Servings</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Servings</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Donation Status</t>
         </is>
@@ -483,35 +478,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>itemno</t>
+          <t>item name</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>item name</t>
+          <t>item type</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>item type</t>
+          <t>calories</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>calories</t>
+          <t xml:space="preserve">amout </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">amout </t>
+          <t>servings</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>servings</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -525,35 +515,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>itemno1</t>
+          <t>itemname1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>itemname1</t>
+          <t>itemtype1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>itemtype1</t>
+          <t>itemcalories1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>itemcalories1</t>
+          <t>itemamount</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>itemamount</t>
+          <t>itemservings1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>itemservings1</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -567,35 +552,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>gffgh1</t>
+          <t>gffh1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gffh1</t>
+          <t>fghfg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>gfhfg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>fghfg</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>gfhfg</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fghfg</t>
+          <t>hfgh</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>hfgh</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -609,35 +589,30 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>hgfh1</t>
+          <t>hfgh1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>hfgh1</t>
+          <t>gfh</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>gfh</t>
+          <t>fgh</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>fgh</t>
+          <t>gfhfg</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>gfhfg</t>
+          <t>hgfh</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>hgfh</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -651,35 +626,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>jhjh1</t>
+          <t>hjhj1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>hjhj1</t>
+          <t>jjjj1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>jjjj1</t>
+          <t>hjjj</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>hjjj</t>
+          <t>jjj</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>jjj</t>
+          <t>jjhj</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>jjhj</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -693,35 +663,30 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>xcv</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>cxvxc</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>xcv</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>cxv</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>xcvcx</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>xcv</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cxvxc</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>xcv</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>cxv</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
-        <is>
-          <t>xcvcx</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -735,35 +700,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cvcx1</t>
+          <t>cxv1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>cxv1</t>
+          <t>xcvcx1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>xcvcx1</t>
+          <t>cxvxc</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>cxvxc</t>
+          <t>cxvx</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>cxvx</t>
+          <t>xcv</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
-        <is>
-          <t>xcv</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -777,35 +737,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cxvx</t>
+          <t>cxv</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>xcv</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>xcv</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>cxv</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>xcv</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>xcv</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>cxv</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
-        <is>
-          <t>cxv</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -819,7 +774,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sddd</t>
+          <t>ddd</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -843,11 +798,6 @@
         </is>
       </c>
       <c r="G10" t="inlineStr">
-        <is>
-          <t>ddd</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -886,11 +836,6 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ggg</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
           <t>accepted</t>
         </is>
       </c>
@@ -928,12 +873,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>kkk</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>pending</t>
+          <t>accepted</t>
         </is>
       </c>
     </row>
@@ -955,7 +895,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>aaa11</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -969,11 +909,6 @@
         </is>
       </c>
       <c r="G13" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
@@ -997,7 +932,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>xxx11</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,11 +946,6 @@
         </is>
       </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -1029,35 +959,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>yyy11</t>
+          <t>yyy1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>yyy11</t>
+          <t>yyy1</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>yyy11</t>
+          <t>yyy1</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>yyy</t>
+          <t>yyy1</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>yyy</t>
+          <t>yyy1</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
-        <is>
-          <t>yyy</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
@@ -1081,7 +1006,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>lll11</t>
+          <t>lll</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1095,11 +1020,6 @@
         </is>
       </c>
       <c r="G16" t="inlineStr">
-        <is>
-          <t>lll</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>
@@ -1113,7 +1033,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>item02</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1138,10 +1058,782 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>kkk1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>kkk1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>kkk1</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>kkk1</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>kkk1</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>yyy</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>yyy</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>yyy</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>yyy</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>yyy</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>zzz1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>zzz1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>zzz1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>zzz1</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>zzz1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>sss1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>sss1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mmm1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>mmm1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>mmm1</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>mmm1</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>mmm1</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>nnn</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>nnn</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>nnn</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>nnn</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>nnn</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>eee111</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>eee111</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>eee111</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>eee111</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>eee111</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>ggg</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>xyxy</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>xyxy</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>xyxy</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>xyxy</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>xyxy</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Pizza</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Non-Veg</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Bread</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Fruits</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Veg Pizza</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Bacon</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Item 7</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Salad</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>accepted</t>
         </is>

</xml_diff>